<commit_message>
Refactor model second try, fix yellow
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TelegramColorMap\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F5064-9788-4B4D-B58B-D0CE63DBAC00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF45FAE2-80CC-4500-8E10-5244863494C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,36 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Color</t>
   </si>
   <si>
     <t>Map</t>
-  </si>
-  <si>
-    <t>Прочитайте книгу - чтение развивает логическое мышление, память и внимание; Съеште 50 грамм грецких орехов - они поднимут Вам настроение; Решите головоломку - решение головоломок всегда положительно воздействует на наш мозг.
-Послушайте любимую музыку - она повысит Вам настроение; Съеште тарелочку гречневой каши - она обеспечит организм и головной мозг энергией; Сложите пазл - это отвлечёт и  поможет расслабиться.
-Отправляйтесь на фотопрогулку - Вы сможете увидеть что-то новое и интересное; Съеште мороженое оно поднимет Вам настроение; Наведите порядок дома и насладитесь результатом.
-Займитесь калиграфией - это Вас успокоит; Выпейте молочный коктель - Вы приободритесь; Сходите на интересующий Вас тренинг - это полезно и увлекательно.
-Посмотрите красивые фото -Вы получите от этого визуальное наслаждение; Съеште салат с сладким перцем - Вы сразу почувствуете прилив сил; Освойте одну полезную привычку.
-Сходите в океанариум - это Вас расслабит; Добавьте в свой рацион шпинат и и другие листовые овощи; Посетите скаладром - это пролезно и увлекательно;
-Посмотрите шоу музакльного фонтана - Вы получите от этого визуальное наслаждение; Съеште орехов - они поднимут Вам настроение Попрыгайте на батуте - это весело и увлекательно.
-Пройдите верёвочный маршрут - это повысит Вам настроение; Выпейте лимонад - Вы приободритесь; Прокатитесь на трамвае - Вы получите от этого визуальное наслаждение.
-Сходите в археологический музей - это познавательно и интересно; Съешьте кусочек тортика - он поднимет Вам настроение; Примите участие в квесте - это занимательно и весело;
-Покрутите халахуп - это укрепит Ваше здоровье; Съешьте мармелад - он поднимет Вам настроение; Приготовьте себе новое блюдо.</t>
-  </si>
-  <si>
-    <t>Займитесь шопингом - Вы получете множество положительных эмоций; Съешьте апельсин - восстановите запасы витамина В9 и улучшите настроение ; Сходите в кино - кино поможет переключиться, разгрузить голову, поднять настроение.
-Поиграйте в видео- или онлайн-игру - это весело и увлекательно; Съешьте авокадо - оно повышает внимание и бдительность; Начните вести свой собственный блог в интернете - Вы приобретете новый опыт.
-Посетите место, в которое давно хотели попасть - это поднимет Вам настроение; Съешьте ягодный мусс - он поднимет Вам настроение; Сделайте доброе дело - это повысит Вашу самооценку .
-Займитесь физическими упражнениями - занятия спортом улучшают наше настроение; Съешьте арбуз - он поднимет Вам настроение; Сделайте то, что раньше никогда не делали - Вы приобретете новый опыт.
-Медитируйте –  это быстрый и эффективный способ расслабиться; Съешьте дыню - она поднимет Вам настроение; Освойте навыки дыхательной гимнастики.
-Сходите на картинг - испытайте чувство экстрима;  Попробуйте одно из блюд итальянской кухни;  Займитесь верховой ездой - иппотерапия благоприятно влияет на наше здороаье.
-Сходите в аквапарк - это весело и интересно; Приготовьте себе авторский бутерброд; Купите лотерейный билет и сорвите джекпот. 
-Поиграйте в настольный теннис - Вы улучшите физическое состояние здоровья; Съешьте халву - она подниме Вам настроение; Сходите в боулинг - это весело и увлекательно.
-Сходите на каток - Вы улучшите физическое состояние здоровья; Съешьте зефир - он поднимет Вам настроение; Поучавствуйте в благотворительной акции - это полезно и благородно.
-Сегодня Вам будут полезны обливания холодной водой из ведра; Выпейте чашку горячего шоколада с хрустящим эклером - это поднимет Вам настроение; Поиграйте в судоку - решение головоломок всегда положительно воздействует на наш мозг.</t>
   </si>
   <si>
     <t>Потанцуйте под энергичный трек - музыка поможет Вам выплеснуть лишнюю энергию; Выпейте чай с ромашкой или мятой - он поможет Вам успокоится; Сходите погулять в парк - это поможет расслабиться и улучшить здоровье.
@@ -64,31 +40,6 @@
 Сходите в караоке - выплесните лишнюю энергию; Выпейте смузи со шпинатом и ананасом - это очень полезно для здоровья; Посадите цветок или дерево около своего дома и ухаживайте.</t>
   </si>
   <si>
-    <t>Сходите в фитнес-клуб - улучшите физическое состояние и найдёте новых друзей; Съеште миндаль - он благотворно влияет на нервную систему; Посмотрите хороший фильм в компании родных или друзей - общайтесь, ведь именно общение делает людей людьми.
-Поиграйте с домашним питомцем - общение с животными улучшает эмоциональное состояние; Побалуйте себя шашлыком - это поднимет Вам настроение; Примите ванну с эфирными маслами - это поможет расслабиться.
-Устройте 20-минутный сеанс йоги или растяжки - это поможет расслабиться; Побалуйте себя чипсами - это повысит Вам настроение; Лягте на диван и помечтайте - разгрузите голову;
-Напишите доброе письмо другу или родственнику; Закажите пиццу - это поднимет Вам настроение; Сделайте кому-нибудь сюрприз.
-Поговорите с самым любимым и отзывчивым близким человеком; Закажите суши - это поднимет Вам настроение; Сделайте кому-нибудь искренний комплимент.
-Покормите уточек, белок или голубей — любую неопасную живность, которую встретите в пределах города; Съешьте цукаты - они повысят Вам настроение; Составьте карту желаний - это расслабляет.
-Обнимите кого-нибудь - физический контакт делает нас счастливее и улучшает состояние здоровья; Съешьте мясной паштет - это сытно и вкусно; Выберетись на природу - расслабьтесь и получите от этого удовольствие.
-Пришлите другу фото: свое, ваше совместное, то, которое напоминает о чем-то приятном; Закажите хачапури - оно поднимет Вам настроение; Сходите с друзьями в кафе - это весело и увлекательно.
-Возьмите карандаши и начните рисовать все, что придет в голову -  просто выразите свое нынешнее настроение; Съешьте шоколадный маффин - он поднимет вам настроение; Улыбнитесь - это лучшее средство для борьбы с плохим настроением;
-Сходите в spa-салон - это полезно для здоровъя; Приготовьте банановый коктейль - он поднимет Вам настроение; Походите босиком по неровной поверхности - это тонизирует и укрепляет нервную систему.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сходите в бассейн - это поможет Вам отдалиться от повседневных проблем и тревог; Съешьте сладкий десерт - сахар поднимает настроение, улучшает работу мозга и дарит заряд энергии; Сходите в контактный зоопарк -общение с животными помогает справиться со стрессом и расслабиться.
-Сделайте перестановку в квартире - этот процесс перезагрузит голову и к Вам придет чувство удовлетворенности. Побалуйте себя и закажите любимую еду на дом - это поднимет Вам настроение;  Покатайтесь на аттракционах в парке развлечений - это поможет Вам вернуться в детство и почувствовать радость и беззаботность.
-Займитесь любимым делом (хобби) - именно любимое дело поможет справиться с негативом; Съешьте что-нибудь из морепродуктов -продукты, богатые витамином D, помогут избавиться от плохого настрония; Примите ванну или контрастный душ - это поможет мгновенно поднять настроение.
-Устройте фотосессию с друзьями - зарядитесь позитивом и получите наслаждение от общения; Выпейте ромашковый чай с ломтиком лимона - это одно из лучших натуральных успокоительных; Покатайтесь на машине по ночному городу - разгрузите голову и обретите  чувство удовлетворения;
-Поэкспериментируйте с внешним видом - это, определённо, поднимет Вам настроение; Приготовьте что-нибудь из помидоров - томаты стабилизируют настроение; Сходите на массаж - расслабтесь и зарядитесь энергией.
-Посмотрите комедию; Съешьте банан - витамины В-группы оказывают более сильное влияние на настроение; Лягте наконец пораньше и выспитесь - это улучшит самочувствие.
-Смейтесь - смех взбодрит вас и уменьшит беспокойство; Приготовьте что-нибудь с морской капустой - она избавляет от хронической усталости и дипрессии; Вспомните все свои достижения - это поможет повысить уверенность в себе.
-Вспомните ситуацию, в которой Вам было особенно хорошо и приятно; Ешьте больше зелени - она полезна для мозга и повышает настроение; Запишите на бумаге все, что беспокоит и выкеньте её.
-Найдите в интернете смешное видео или анекдоты; Выпейте чашку кофе - он ободряет и поднимает настроение; Подойдите к зеркалу и скажите себе 3 комплимента - это поможет повысить самооценку.
-Прочитайте анекдоты; Выпейте чашку черного чая - он поднимет Вам настроение; Вспомните приятные моменты из жизни.
-</t>
-  </si>
-  <si>
     <t>Сходите в бассейн - это поможет Вам отдалиться от повседневных проблем и тревог; Съешьте сладкий десерт - сахар поднимает настроение, улучшает работу мозга и дарит заряд энергии; Сходите в контактный зоопарк -общение с животными помогает справиться со стрессом и расслабиться.
 Сделайте перестановку в квартире - этот процесс перезагрузит голову и к Вам придет чувство удовлетворенности. Побалуйте себя и закажите любимую еду на дом - это поднимет Вам настроение;  Покатайтесь на аттракционах в парке развлечений - это поможет Вам вернуться в детство и почувствовать радость и беззаботность.
 Займитесь любимым делом (хобби) - именно любимое дело поможет справиться с негативом; Съешьте что-нибудь из морепродуктов -продукты, богатые витамином D, помогут избавиться от плохого настрония; Примите ванну или контрастный душ - это поможет мгновенно поднять настроение.
@@ -113,9 +64,6 @@
     <t>red</t>
   </si>
   <si>
-    <t>yelow</t>
-  </si>
-  <si>
     <t>violet</t>
   </si>
   <si>
@@ -126,6 +74,70 @@
   </si>
   <si>
     <t>white</t>
+  </si>
+  <si>
+    <t>Займитесь шопингом - Вы получете множество положительных эмоций; Съешьте апельсин - восстановите запасы витамина В9 и улучшите настроение ; Сходите в кино - кино поможет переключиться, разгрузить голову, поднять настроение.
+Поиграйте в видео- или онлайн-игру - это весело и увлекательно; Съешьте авокадо - оно повышает внимание и бдительность; Начните вести свой собственный блог в интернете - Вы приобретете новый опыт.
+Посетите место, в которое давно хотели попасть - это поднимет Вам настроение; Съешьте ягодный мусс - он поднимет Вам настроение; Сделайте доброе дело - это повысит Вашу самооценку .
+Займитесь физическими упражнениями - занятия спортом улучшают наше настроение; Съешьте арбуз - он поднимет Вам настроение; Сделайте то, что раньше никогда не делали - Вы приобретете новый опыт.
+Медитируйте –  это быстрый и эффективный способ расслабиться; Съешьте дыню - она поднимет Вам настроение; Освойте навыки дыхательной гимнастики.
+Сходите на картинг - испытайте чувство экстрима;  Попробуйте одно из блюд итальянской кухни;  Займитесь верховой ездой - иппотерапия благоприятно влияет на наше здоровье.
+Сходите в аквапарк - это весело и интересно; Приготовьте себе авторский бутерброд; Купите лотерейный билет и сорвите джекпот. 
+Поиграйте в настольный теннис - Вы улучшите физическое состояние здоровья; Съешьте халву - она подниме Вам настроение; Сходите в боулинг - это весело и увлекательно.
+Сходите на каток - Вы улучшите физическое состояние здоровья; Съешьте зефир - он поднимет Вам настроение; Поучавствуйте в благотворительной акции - это полезно и благородно.
+Сегодня Вам будут полезны обливания холодной водой из ведра; Выпейте чашку горячего шоколада с хрустящим эклером - это поднимет Вам настроение; Поиграйте в судоку - решение головоломок всегда положительно воздействует на наш мозг.</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>Сходите в фитнес-клуб - улучшите физическое состояние и найдёте новых друзей; Съеште миндаль - он благотворно влияет на нервную систему; Посмотрите хороший фильм в компании родных или друзей - общайтесь, ведь именно общение делает людей людьми.
+Поиграйте с домашним питомцем - общение с животными улучшает эмоциональное состояние; Побалуйте себя шашлыком - это поднимет Вам настроение; Примите ванну с эфирными маслами - это поможет расслабиться.
+Устройте 20-минутный сеанс йоги или растяжки - это поможет расслабиться; Побалуйте себя чипсами - это повысит Вам настроение; Лягте на диван и помечтайте - разгрузите голову.
+Напишите доброе письмо другу или родственнику; Закажите пиццу - это поднимет Вам настроение; Сделайте кому-нибудь сюрприз.
+Поговорите с самым любимым и отзывчивым близким человеком; Закажите суши - это поднимет Вам настроение; Сделайте кому-нибудь искренний комплимент.
+Покормите уточек, белок или голубей — любую неопасную живность, которую встретите в пределах города; Съешьте цукаты - они повысят Вам настроение; Составьте карту желаний - это расслабляет.
+Обнимите кого-нибудь - физический контакт делает нас счастливее и улучшает состояние здоровья; Съешьте мясной паштет - это сытно и вкусно; Выберетись на природу - расслабьтесь и получите от этого удовольствие.
+Пришлите другу фото: свое, ваше совместное, то, которое напоминает о чем-то приятном; Закажите хачапури - оно поднимет Вам настроение; Сходите с друзьями в кафе - это весело и увлекательно.
+Возьмите карандаши и начните рисовать все, что придет в голову -  просто выразите свое нынешнее настроение; Съешьте шоколадный маффин - он поднимет вам настроение; Улыбнитесь - это лучшее средство для борьбы с плохим настроением.
+Сходите в spa-салон - это полезно для здоровъя; Приготовьте банановый коктейль - он поднимет Вам настроение; Походите босиком по неровной поверхности - это тонизирует и укрепляет нервную систему.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сходите в бассейн - это поможет Вам отдалиться от повседневных проблем и тревог; Съешьте сладкий десерт - сахар поднимает настроение, улучшает работу мозга и дарит заряд энергии; Сходите в контактный зоопарк -общение с животными помогает справиться со стрессом и расслабиться.
+Сделайте перестановку в квартире - этот процесс перезагрузит голову и к Вам придет чувство удовлетворенности; Побалуйте себя и закажите любимую еду на дом - это поднимет Вам настроение;  Покатайтесь на аттракционах в парке развлечений - это поможет Вам вернуться в детство и почувствовать радость и беззаботность.
+Займитесь любимым делом (хобби) - именно любимое дело поможет справиться с негативом; Съешьте что-нибудь из морепродуктов -продукты, богатые витамином D, помогут избавиться от плохого настрония; Примите ванну или контрастный душ - это поможет мгновенно поднять настроение.
+Устройте фотосессию с друзьями - зарядитесь позитивом и получите наслаждение от общения; Выпейте ромашковый чай с ломтиком лимона - это одно из лучших натуральных успокоительных; Покатайтесь на машине по ночному городу - разгрузите голову и обретите  чувство удовлетворения;
+Поэкспериментируйте с внешним видом - это, определённо, поднимет Вам настроение; Приготовьте что-нибудь из помидоров - томаты стабилизируют настроение; Сходите на массаж - расслабтесь и зарядитесь энергией.
+Посмотрите комедию; Съешьте банан - витамины В-группы оказывают более сильное влияние на настроение; Лягте наконец пораньше и выспитесь - это улучшит самочувствие.
+Смейтесь - смех взбодрит вас и уменьшит беспокойство; Приготовьте что-нибудь с морской капустой - она избавляет от хронической усталости и дипрессии; Вспомните все свои достижения - это поможет повысить уверенность в себе.
+Вспомните ситуацию, в которой Вам было особенно хорошо и приятно; Ешьте больше зелени - она полезна для мозга и повышает настроение; Запишите на бумаге все, что беспокоит и выкеньте её.
+Найдите в интернете смешное видео или анекдоты; Выпейте чашку кофе - он ободряет и поднимает настроение; Подойдите к зеркалу и скажите себе 3 комплимента - это поможет повысить самооценку.
+Прочитайте анекдоты; Выпейте чашку черного чая - он поднимет Вам настроение; Вспомните приятные моменты из жизни.
+</t>
+  </si>
+  <si>
+    <t>Потанцуйте под энергичный трек - музыка поможет Вам выплеснуть лишнюю энергию; Выпейте чай с ромашкой или мятой - он поможет Вам успокоится; Сходите погулять в парк - это поможет расслабиться и улучшить здоровье.
+Спойте любимую зажигательную песню - выплесните лишнюю энергию; Выпейте стакан воды - вода помогает успокоиться; Позвоните другу и поболтайте с ним.
+Выпустите пар и покричите; Ешьте фасоль и другие бобовые - они помогаю успокоиться; Прокатитесь незнакомым маршрутом общественного транспорта и разглядывайте город из окна - это позновательно и интересно.
+Сходте погулять в парк - прогулки снижают уровень стресса, укрепляют общий иммунитет, повышают настроение; Съешьте несколько кусочков темного шоколада - он помогает улучшить эмоциональное состояние; Поиграйте в дартс.
+Устройте уборку - выплесните эмоции, а после насладитесь результатом;  Добавьте в свой рацион питания козий сыр - он успакаивает и полезен для головного мозга; Сходите на прогулку к водоему и расслабьтесь.
+Понаблюдайте за язычками пламени на свечках - это успокоит ваш ум и расслабит вас; Выпейте чай с мелиссой - он успакоет Вас; Поиграйте в баскетбол - выплесните лишнюю энергию.
+Представьте море, солнце, пальмы, теплый ветер и насладитесь блаженством; Выпейте виноградный сок - он поможет расслабиться; Займитесь аквааэробикой - выплесните лишнюю энергию.
+Сходите в тир и постреляйте из лука - выплесните лишнюю энергию; Выпейте грейпфрутовый фреш - он поможет Вам расслабиться;  Поиграйте в волейбол -это весело и увлекательно.
+Займитесь фехтованием - это поможет расслабиться; Выпейте фруктовый кисель - он успокоит Вас; Покатайтесь на велосипеде - это полезно для здоровья.
+Сходите в караоке - выплесните лишнюю энергию; Выпейте смузи со шпинатом и ананасом - это очень полезно для здоровья; Посадите цветок или дерево около своего дома и ухаживайте.</t>
+  </si>
+  <si>
+    <t>Прочитайте книгу - чтение развивает логическое мышление, память и внимание; Съеште 50 грамм грецких орехов - они поднимут Вам настроение; Решите головоломку - решение головоломок всегда положительно воздействует на наш мозг.
+Послушайте любимую музыку - она повысит Вам настроение; Съеште тарелочку гречневой каши - она обеспечит организм и головной мозг энергией; Сложите пазл - это отвлечёт и  поможет расслабиться.
+Отправляйтесь на фотопрогулку - Вы сможете увидеть что-то новое и интересное; Съеште мороженое оно поднимет Вам настроение; Наведите порядок дома и насладитесь результатом.
+Займитесь калиграфией - это Вас успокоит; Выпейте молочный коктель - Вы приободритесь; Сходите на интересующий Вас тренинг - это полезно и увлекательно.
+Посмотрите красивые фото -Вы получите от этого визуальное наслаждение; Съеште салат с сладким перцем - Вы сразу почувствуете прилив сил; Освойте одну полезную привычку.
+Сходите в океанариум - это Вас расслабит; Добавьте в свой рацион шпинат и и другие листовые овощи; Посетите скаладром - это пролезно и увлекательно.
+Посмотрите шоу музакльного фонтана - Вы получите от этого визуальное наслаждение; Съеште орехов - они поднимут Вам настроение; Попрыгайте на батуте - это весело и увлекательно.
+Пройдите верёвочный маршрут - это повысит Вам настроение; Выпейте лимонад - Вы приободритесь; Прокатитесь на трамвае - Вы получите от этого визуальное наслаждение.
+Сходите в археологический музей - это познавательно и интересно; Съешьте кусочек тортика - он поднимет Вам настроение; Примите участие в квесте - это занимательно и весело.
+Покрутите халахуп - это укрепит Ваше здоровье; Съешьте мармелад - он поднимет Вам настроение; Приготовьте себе новое блюдо</t>
   </si>
 </sst>
 </file>
@@ -532,11 +544,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="182.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -546,103 +561,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="285" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix for last time(i hope) dataset and reteaching tree. A little bit change color dict
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TelegramColorMap\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF45FAE2-80CC-4500-8E10-5244863494C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA36529-6BB0-45A6-8E1D-6F407ABC742D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,30 +28,6 @@
     <t>Map</t>
   </si>
   <si>
-    <t>Потанцуйте под энергичный трек - музыка поможет Вам выплеснуть лишнюю энергию; Выпейте чай с ромашкой или мятой - он поможет Вам успокоится; Сходите погулять в парк - это поможет расслабиться и улучшить здоровье.
-Спойте любимую зажигательную песню - выплесните лишнюю энергию. Выпейте стакан воды - вода помогает успокоиться; Позвоните другу и поболтайте с ним.
-Выпустите пар и покричите; Ешьте фасоль и другие бобовые - они помогаю успокоиться; Прокатитесь незнакомым маршрутом общественного транспорта и разглядывайте город из окна - это позновательно и интересно.
-Сходте погулять в парк - прогулки снижают уровень стресса, укрепляют общий иммунитет, повышают настроение; Съешьте несколько кусочков темного шоколада - он помогает улучшить эмоциональное состояние; Поиграйте в дартс.
-Устройте уборку - выплесните эмоции, а после насладитесь результатом;  Добавьте в свой рацион питания козий сыр - он успакаивает и полезен для головного мозга; Сходите на прогулку к водоему и расслабьтесь.
-Понаблюдайте за язычками пламени на свечках - это успокоит ваш ум и расслабит вас; Выпейте чай с мелиссой - он успакоет Вас; Поиграйте в баскетбол - выплесните лишнюю энергию.
-Представьте море, солнце, пальмы, теплый ветер и насладитесь блаженством; Выпейте виноградный сок - он поможет расслабиться; Займитесь аквааэробикой - выплесните лишнюю энергию.
-Сходите в тир и постреляйте из лука - выплесните лишнюю энергию; Выпейте грейпфрутовый фреш - он поможет Вам расслабиться;  Поиграйте в волейбол -это весело и увлекательно.
-Займитесь фехтованием - это поможет расслабиться; Выпейте фруктовый кисель - он успокоит Вас; Покатайтесь на велосипеде - это полезно для здоровья.
-Сходите в караоке - выплесните лишнюю энергию; Выпейте смузи со шпинатом и ананасом - это очень полезно для здоровья; Посадите цветок или дерево около своего дома и ухаживайте.</t>
-  </si>
-  <si>
-    <t>Сходите в бассейн - это поможет Вам отдалиться от повседневных проблем и тревог; Съешьте сладкий десерт - сахар поднимает настроение, улучшает работу мозга и дарит заряд энергии; Сходите в контактный зоопарк -общение с животными помогает справиться со стрессом и расслабиться.
-Сделайте перестановку в квартире - этот процесс перезагрузит голову и к Вам придет чувство удовлетворенности. Побалуйте себя и закажите любимую еду на дом - это поднимет Вам настроение;  Покатайтесь на аттракционах в парке развлечений - это поможет Вам вернуться в детство и почувствовать радость и беззаботность.
-Займитесь любимым делом (хобби) - именно любимое дело поможет справиться с негативом; Съешьте что-нибудь из морепродуктов -продукты, богатые витамином D, помогут избавиться от плохого настрония; Примите ванну или контрастный душ - это поможет мгновенно поднять настроение.
-Устройте фотосессию с друзьями - зарядитесь позитивом и получите наслаждение от общения; Выпейте ромашковый чай с ломтиком лимона - это одно из лучших натуральных успокоительных; Покатайтесь на машине по ночному городу - разгрузите голову и обретите  чувство удовлетворения;
-Поэкспериментируйте с внешним видом - это, определённо, поднимет Вам настроение; Приготовьте что-нибудь из помидоров - томаты стабилизируют настроение; Сходите на массаж - расслабтесь и зарядитесь энергией.
-Посмотрите комедию; Съешьте банан - витамины В-группы оказывают более сильное влияние на настроение; Лягте наконец пораньше и выспитесь - это улучшит самочувствие.
-Смейтесь - смех взбодрит вас и уменьшит беспокойство; Приготовьте что-нибудь с морской капустой - она избавляет от хронической усталости и дипрессии; Вспомните все свои достижения - это поможет повысить уверенность в себе.
-Вспомните ситуацию, в которой Вам было особенно хорошо и приятно; Ешьте больше зелени - она полезна для мозга и повышает настроение; Запишите на бумаге все, что беспокоит и выкеньте её.
-Найдите в интернете смешное видео или анекдоты; Выпейте чашку кофе - он ободряет и поднимает настроение; Подойдите к зеркалу и скажите себе 3 комплимента - это поможет повысить самооценку.
-Прочитайте анекдоты; Выпейте чашку черного чая - он поднимет Вам настроение; Вспомните приятные моменты из жизни.</t>
-  </si>
-  <si>
     <t>blue</t>
   </si>
   <si>
@@ -76,44 +52,7 @@
     <t>white</t>
   </si>
   <si>
-    <t>Займитесь шопингом - Вы получете множество положительных эмоций; Съешьте апельсин - восстановите запасы витамина В9 и улучшите настроение ; Сходите в кино - кино поможет переключиться, разгрузить голову, поднять настроение.
-Поиграйте в видео- или онлайн-игру - это весело и увлекательно; Съешьте авокадо - оно повышает внимание и бдительность; Начните вести свой собственный блог в интернете - Вы приобретете новый опыт.
-Посетите место, в которое давно хотели попасть - это поднимет Вам настроение; Съешьте ягодный мусс - он поднимет Вам настроение; Сделайте доброе дело - это повысит Вашу самооценку .
-Займитесь физическими упражнениями - занятия спортом улучшают наше настроение; Съешьте арбуз - он поднимет Вам настроение; Сделайте то, что раньше никогда не делали - Вы приобретете новый опыт.
-Медитируйте –  это быстрый и эффективный способ расслабиться; Съешьте дыню - она поднимет Вам настроение; Освойте навыки дыхательной гимнастики.
-Сходите на картинг - испытайте чувство экстрима;  Попробуйте одно из блюд итальянской кухни;  Займитесь верховой ездой - иппотерапия благоприятно влияет на наше здоровье.
-Сходите в аквапарк - это весело и интересно; Приготовьте себе авторский бутерброд; Купите лотерейный билет и сорвите джекпот. 
-Поиграйте в настольный теннис - Вы улучшите физическое состояние здоровья; Съешьте халву - она подниме Вам настроение; Сходите в боулинг - это весело и увлекательно.
-Сходите на каток - Вы улучшите физическое состояние здоровья; Съешьте зефир - он поднимет Вам настроение; Поучавствуйте в благотворительной акции - это полезно и благородно.
-Сегодня Вам будут полезны обливания холодной водой из ведра; Выпейте чашку горячего шоколада с хрустящим эклером - это поднимет Вам настроение; Поиграйте в судоку - решение головоломок всегда положительно воздействует на наш мозг.</t>
-  </si>
-  <si>
     <t>yellow</t>
-  </si>
-  <si>
-    <t>Сходите в фитнес-клуб - улучшите физическое состояние и найдёте новых друзей; Съеште миндаль - он благотворно влияет на нервную систему; Посмотрите хороший фильм в компании родных или друзей - общайтесь, ведь именно общение делает людей людьми.
-Поиграйте с домашним питомцем - общение с животными улучшает эмоциональное состояние; Побалуйте себя шашлыком - это поднимет Вам настроение; Примите ванну с эфирными маслами - это поможет расслабиться.
-Устройте 20-минутный сеанс йоги или растяжки - это поможет расслабиться; Побалуйте себя чипсами - это повысит Вам настроение; Лягте на диван и помечтайте - разгрузите голову.
-Напишите доброе письмо другу или родственнику; Закажите пиццу - это поднимет Вам настроение; Сделайте кому-нибудь сюрприз.
-Поговорите с самым любимым и отзывчивым близким человеком; Закажите суши - это поднимет Вам настроение; Сделайте кому-нибудь искренний комплимент.
-Покормите уточек, белок или голубей — любую неопасную живность, которую встретите в пределах города; Съешьте цукаты - они повысят Вам настроение; Составьте карту желаний - это расслабляет.
-Обнимите кого-нибудь - физический контакт делает нас счастливее и улучшает состояние здоровья; Съешьте мясной паштет - это сытно и вкусно; Выберетись на природу - расслабьтесь и получите от этого удовольствие.
-Пришлите другу фото: свое, ваше совместное, то, которое напоминает о чем-то приятном; Закажите хачапури - оно поднимет Вам настроение; Сходите с друзьями в кафе - это весело и увлекательно.
-Возьмите карандаши и начните рисовать все, что придет в голову -  просто выразите свое нынешнее настроение; Съешьте шоколадный маффин - он поднимет вам настроение; Улыбнитесь - это лучшее средство для борьбы с плохим настроением.
-Сходите в spa-салон - это полезно для здоровъя; Приготовьте банановый коктейль - он поднимет Вам настроение; Походите босиком по неровной поверхности - это тонизирует и укрепляет нервную систему.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сходите в бассейн - это поможет Вам отдалиться от повседневных проблем и тревог; Съешьте сладкий десерт - сахар поднимает настроение, улучшает работу мозга и дарит заряд энергии; Сходите в контактный зоопарк -общение с животными помогает справиться со стрессом и расслабиться.
-Сделайте перестановку в квартире - этот процесс перезагрузит голову и к Вам придет чувство удовлетворенности; Побалуйте себя и закажите любимую еду на дом - это поднимет Вам настроение;  Покатайтесь на аттракционах в парке развлечений - это поможет Вам вернуться в детство и почувствовать радость и беззаботность.
-Займитесь любимым делом (хобби) - именно любимое дело поможет справиться с негативом; Съешьте что-нибудь из морепродуктов -продукты, богатые витамином D, помогут избавиться от плохого настрония; Примите ванну или контрастный душ - это поможет мгновенно поднять настроение.
-Устройте фотосессию с друзьями - зарядитесь позитивом и получите наслаждение от общения; Выпейте ромашковый чай с ломтиком лимона - это одно из лучших натуральных успокоительных; Покатайтесь на машине по ночному городу - разгрузите голову и обретите  чувство удовлетворения;
-Поэкспериментируйте с внешним видом - это, определённо, поднимет Вам настроение; Приготовьте что-нибудь из помидоров - томаты стабилизируют настроение; Сходите на массаж - расслабтесь и зарядитесь энергией.
-Посмотрите комедию; Съешьте банан - витамины В-группы оказывают более сильное влияние на настроение; Лягте наконец пораньше и выспитесь - это улучшит самочувствие.
-Смейтесь - смех взбодрит вас и уменьшит беспокойство; Приготовьте что-нибудь с морской капустой - она избавляет от хронической усталости и дипрессии; Вспомните все свои достижения - это поможет повысить уверенность в себе.
-Вспомните ситуацию, в которой Вам было особенно хорошо и приятно; Ешьте больше зелени - она полезна для мозга и повышает настроение; Запишите на бумаге все, что беспокоит и выкеньте её.
-Найдите в интернете смешное видео или анекдоты; Выпейте чашку кофе - он ободряет и поднимает настроение; Подойдите к зеркалу и скажите себе 3 комплимента - это поможет повысить самооценку.
-Прочитайте анекдоты; Выпейте чашку черного чая - он поднимет Вам настроение; Вспомните приятные моменты из жизни.
-</t>
   </si>
   <si>
     <t>Потанцуйте под энергичный трек - музыка поможет Вам выплеснуть лишнюю энергию; Выпейте чай с ромашкой или мятой - он поможет Вам успокоится; Сходите погулять в парк - это поможет расслабиться и улучшить здоровье.
@@ -138,6 +77,66 @@
 Пройдите верёвочный маршрут - это повысит Вам настроение; Выпейте лимонад - Вы приободритесь; Прокатитесь на трамвае - Вы получите от этого визуальное наслаждение.
 Сходите в археологический музей - это познавательно и интересно; Съешьте кусочек тортика - он поднимет Вам настроение; Примите участие в квесте - это занимательно и весело.
 Покрутите халахуп - это укрепит Ваше здоровье; Съешьте мармелад - он поднимет Вам настроение; Приготовьте себе новое блюдо</t>
+  </si>
+  <si>
+    <t>Займитесь шопингом - Вы получете множество положительных эмоций; Съешьте апельсин - восстановите запасы витамина В9 и улучшите настроение ; Сходите в кино - кино поможет переключиться, разгрузить голову, поднять настроение.
+Поиграйте в видео- или онлайн-игру - это весело и увлекательно; Съешьте авокадо - оно повышает внимание и бдительность; Начните вести свой собственный блог в интернете - Вы приобретете новый опыт.
+Посетите место, в которое давно хотели попасть - это поднимет Вам настроение; Съешьте ягодный мусс - он поднимет Вам настроение; Сделайте доброе дело - это повысит Вашу самооценку .
+Займитесь физическими упражнениями - занятия спортом улучшают наше настроение; Съешьте арбуз - он поднимет Вам настроение; Сделайте то, что раньше никогда не делали - Вы приобретете новый опыт.
+Медитируйте –  это быстрый и эффективный способ расслабиться; Съешьте дыню - она поднимет Вам настроение; Освойте навыки дыхательной гимнастики.
+Сходите на картинг - испытайте чувство экстрима;  Попробуйте одно из блюд итальянской кухни;  Займитесь верховой ездой - иппотерапия благоприятно влияет на наше здоровье.
+Сходите в аквапарк - это весело и интересно; Приготовьте себе авторский бутерброд; Купите лотерейный билет и сорвите джекпот. 
+Поиграйте в настольный теннис - Вы улучшите физическое состояние здоровья; Съешьте халву - она подниме Вам настроение; Сходите в боулинг - это весело и увлекательно.
+Сходите на каток - Вы улучшите физическое состояние здоровья; Съешьте зефир - он поднимет Вам настроение; Поучавствуйте в благотворительной акции - это полезно и благородно.
+Сегодня Вам будут полезны обливания холодной водой из ведра; Выпейте чашку горячего шоколада с хрустящим эклером - это поднимет Вам настроение; Поиграйте в судоку - решение головоломок всегда положительно воздействует на наш мозг</t>
+  </si>
+  <si>
+    <t>Потанцуйте под энергичный трек - музыка поможет Вам выплеснуть лишнюю энергию; Выпейте чай с ромашкой или мятой - он поможет Вам успокоится; Сходите погулять в парк - это поможет расслабиться и улучшить здоровье.
+Спойте любимую зажигательную песню - выплесните лишнюю энергию; Выпейте стакан воды - вода помогает успокоиться; Позвоните другу и поболтайте с ним.
+Выпустите пар и покричите; Ешьте фасоль и другие бобовые - они помогаю успокоиться; Прокатитесь незнакомым маршрутом общественного транспорта и разглядывайте город из окна - это позновательно и интересно.
+Сходте погулять в парк - прогулки снижают уровень стресса, укрепляют общий иммунитет, повышают настроение; Съешьте несколько кусочков темного шоколада - он помогает улучшить эмоциональное состояние; Поиграйте в дартс.
+Устройте уборку - выплесните эмоции, а после насладитесь результатом;  Добавьте в свой рацион питания козий сыр - он успакаивает и полезен для головного мозга; Сходите на прогулку к водоему и расслабьтесь.
+Понаблюдайте за язычками пламени на свечках - это успокоит ваш ум и расслабит вас; Выпейте чай с мелиссой - он успакоет Вас; Поиграйте в баскетбол - выплесните лишнюю энергию.
+Представьте море, солнце, пальмы, теплый ветер и насладитесь блаженством; Выпейте виноградный сок - он поможет расслабиться; Займитесь аквааэробикой - выплесните лишнюю энергию.
+Сходите в тир и постреляйте из лука - выплесните лишнюю энергию; Выпейте грейпфрутовый фреш - он поможет Вам расслабиться;  Поиграйте в волейбол -это весело и увлекательно.
+Займитесь фехтованием - это поможет расслабиться; Выпейте фруктовый кисель - он успокоит Вас; Покатайтесь на велосипеде - это полезно для здоровья.
+Сходите в караоке - выплесните лишнюю энергию; Выпейте смузи со шпинатом и ананасом - это очень полезно для здоровья; Посадите цветок или дерево около своего дома и ухаживайте</t>
+  </si>
+  <si>
+    <t>Сходите в фитнес-клуб - улучшите физическое состояние и найдёте новых друзей; Съеште миндаль - он благотворно влияет на нервную систему; Посмотрите хороший фильм в компании родных или друзей - общайтесь, ведь именно общение делает людей людьми.
+Поиграйте с домашним питомцем - общение с животными улучшает эмоциональное состояние; Побалуйте себя шашлыком - это поднимет Вам настроение; Примите ванну с эфирными маслами - это поможет расслабиться.
+Устройте 20-минутный сеанс йоги или растяжки - это поможет расслабиться; Побалуйте себя чипсами - это повысит Вам настроение; Лягте на диван и помечтайте - разгрузите голову.
+Напишите доброе письмо другу или родственнику; Закажите пиццу - это поднимет Вам настроение; Сделайте кому-нибудь сюрприз.
+Поговорите с самым любимым и отзывчивым близким человеком; Закажите суши - это поднимет Вам настроение; Сделайте кому-нибудь искренний комплимент.
+Покормите уточек, белок или голубей — любую неопасную живность, которую встретите в пределах города; Съешьте цукаты - они повысят Вам настроение; Составьте карту желаний - это расслабляет.
+Обнимите кого-нибудь - физический контакт делает нас счастливее и улучшает состояние здоровья; Съешьте мясной паштет - это сытно и вкусно; Выберетись на природу - расслабьтесь и получите от этого удовольствие.
+Пришлите другу фото: свое, ваше совместное, то, которое напоминает о чем-то приятном; Закажите хачапури - оно поднимет Вам настроение; Сходите с друзьями в кафе - это весело и увлекательно.
+Возьмите карандаши и начните рисовать все, что придет в голову -  просто выразите свое нынешнее настроение; Съешьте шоколадный маффин - он поднимет вам настроение; Улыбнитесь - это лучшее средство для борьбы с плохим настроением.
+Сходите в spa-салон - это полезно для здоровъя; Приготовьте банановый коктейль - он поднимет Вам настроение; Походите босиком по неровной поверхности - это тонизирует и укрепляет нервную систему</t>
+  </si>
+  <si>
+    <t>Сходите в бассейн - это поможет Вам отдалиться от повседневных проблем и тревог; Съешьте сладкий десерт - сахар поднимает настроение, улучшает работу мозга и дарит заряд энергии; Сходите в контактный зоопарк -общение с животными помогает справиться со стрессом и расслабиться.
+Сделайте перестановку в квартире - этот процесс перезагрузит голову и к Вам придет чувство удовлетворенности; Побалуйте себя и закажите любимую еду на дом - это поднимет Вам настроение;  Покатайтесь на аттракционах в парке развлечений - это поможет Вам вернуться в детство и почувствовать радость и беззаботность.
+Займитесь любимым делом (хобби) - именно любимое дело поможет справиться с негативом; Съешьте что-нибудь из морепродуктов -продукты, богатые витамином D, помогут избавиться от плохого настрония; Примите ванну или контрастный душ - это поможет мгновенно поднять настроение.
+Устройте фотосессию с друзьями - зарядитесь позитивом и получите наслаждение от общения; Выпейте ромашковый чай с ломтиком лимона - это одно из лучших натуральных успокоительных; Покатайтесь на машине по ночному городу - разгрузите голову и обретите  чувство удовлетворения.
+Поэкспериментируйте с внешним видом - это, определённо, поднимет Вам настроение; Приготовьте что-нибудь из помидоров - томаты стабилизируют настроение; Сходите на массаж - расслабтесь и зарядитесь энергией.
+Посмотрите комедию; Съешьте банан - витамины В-группы оказывают более сильное влияние на настроение; Лягте наконец пораньше и выспитесь - это улучшит самочувствие.
+Смейтесь - смех взбодрит вас и уменьшит беспокойство; Приготовьте что-нибудь с морской капустой - она избавляет от хронической усталости и дипрессии; Вспомните все свои достижения - это поможет повысить уверенность в себе.
+Вспомните ситуацию, в которой Вам было особенно хорошо и приятно; Ешьте больше зелени - она полезна для мозга и повышает настроение; Запишите на бумаге все, что беспокоит и выкеньте её.
+Найдите в интернете смешное видео или анекдоты; Выпейте чашку кофе - он ободряет и поднимает настроение; Подойдите к зеркалу и скажите себе 3 комплимента - это поможет повысить самооценку.
+Прочитайте анекдоты; Выпейте чашку черного чая - он поднимет Вам настроение; Вспомните приятные моменты из жизни</t>
+  </si>
+  <si>
+    <t>Сходите в бассейн - это поможет Вам отдалиться от повседневных проблем и тревог; Съешьте сладкий десерт - сахар поднимает настроение, улучшает работу мозга и дарит заряд энергии; Сходите в контактный зоопарк -общение с животными помогает справиться со стрессом и расслабиться.
+Сделайте перестановку в квартире - этот процесс перезагрузит голову и к Вам придет чувство удовлетворенности; Побалуйте себя и закажите любимую еду на дом - это поднимет Вам настроение;  Покатайтесь на аттракционах в парке развлечений - это поможет Вам вернуться в детство и почувствовать радость и беззаботность.
+Займитесь любимым делом (хобби) - именно любимое дело поможет справиться с негативом; Съешьте что-нибудь из морепродуктов -продукты, богатые витамином D, помогут избавиться от плохого настрония; Примите ванну или контрастный душ - это поможет мгновенно поднять настроение.
+Устройте фотосессию с друзьями - зарядитесь позитивом и получите наслаждение от общения; Выпейте ромашковый чай с ломтиком лимона - это одно из лучших натуральных успокоительных; Покатайтесь на машине по ночному городу - разгрузите голову и обретите  чувство удовлетворения.
+Поэкспериментируйте с внешним видом - это, определённо, поднимет Вам настроение; Приготовьте что-нибудь из помидоров - томаты стабилизируют настроение; Сходите на массаж - расслабьтесь и зарядитесь энергией.
+Посмотрите комедию; Съешьте банан - витамины В-группы оказывают более сильное влияние на настроение; Лягте наконец пораньше и выспитесь - это улучшит самочувствие.
+Смейтесь - смех взбодрит вас и уменьшит беспокойство; Приготовьте что-нибудь с морской капустой - она избавляет от хронической усталости и дипрессии; Вспомните все свои достижения - это поможет повысить уверенность в себе.
+Вспомните ситуацию, в которой Вам было особенно хорошо и приятно; Ешьте больше зелени - она полезна для мозга и повышает настроение; Запишите на бумаге все, что беспокоит и выкеньте её.
+Найдите в интернете смешное видео или анекдоты; Выпейте чашку кофе - он ободряет и поднимает настроение; Подойдите к зеркалу и скажите себе 3 комплимента - это поможет повысить самооценку.
+Прочитайте анекдоты; Выпейте чашку черного чая - он поднимет Вам настроение; Вспомните приятные моменты из жизни</t>
   </si>
 </sst>
 </file>
@@ -544,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,10 +565,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="225" x14ac:dyDescent="0.25">
@@ -577,10 +576,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="225" x14ac:dyDescent="0.25">
@@ -588,10 +587,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -599,10 +598,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="255" x14ac:dyDescent="0.25">
@@ -610,21 +609,21 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="270" x14ac:dyDescent="0.25">
@@ -632,10 +631,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="270" x14ac:dyDescent="0.25">
@@ -643,10 +642,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="270" x14ac:dyDescent="0.25">
@@ -654,10 +653,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>